<commit_message>
update BOM brake system
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/BR/BRA0100_to_BRA0200.xlsx
+++ b/CR - Cost Report/BOM/BR/BRA0100_to_BRA0200.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EPSA_git\STUF2019\CR - Cost Report\BOM\BR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4733032F-3D9D-4EE7-8F3E-05BCD58E608A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EF4EC-9C06-4992-A2FF-FB84036D0681}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>Béringer 2D1, dual piston 27mm bore</t>
   </si>
   <si>
-    <t>Button</t>
-  </si>
-  <si>
     <t>to assemble Brake rotor and shrink disc</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>BR_02005</t>
+  </si>
+  <si>
+    <t>Rotor button</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -716,38 +716,38 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="4">
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -826,38 +826,38 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="4">
         <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="F13" s="5">
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction BR 1 / 2
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/BR/BRA0100_to_BRA0200.xlsx
+++ b/CR - Cost Report/BOM/BR/BRA0100_to_BRA0200.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EPSA_git\STUF2019\CR - Cost Report\BOM\BR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\BR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24EF4EC-9C06-4992-A2FF-FB84036D0681}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -177,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,27 +596,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.68359375" customWidth="1"/>
-    <col min="2" max="2" width="26.20703125" customWidth="1"/>
-    <col min="3" max="3" width="22.3125" customWidth="1"/>
-    <col min="4" max="4" width="23.3125" customWidth="1"/>
-    <col min="5" max="5" width="44.41796875" customWidth="1"/>
-    <col min="6" max="6" width="14.7890625" customWidth="1"/>
-    <col min="7" max="7" width="16.89453125" customWidth="1"/>
-    <col min="8" max="8" width="11.5234375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -655,7 +654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -674,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -693,7 +692,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
@@ -712,7 +711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -731,7 +730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -750,7 +749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -765,7 +764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -784,7 +783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
@@ -803,7 +802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -822,7 +821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -841,7 +840,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">

</xml_diff>